<commit_message>
Cronograma de proyecto creado v2
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Desktop\Universidad\ciclo IX\Gestión de  Configuración y Mantenimiento\Proyecto\WebSecurity\WebSecurity\DESARROLLO\PWCEV\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3041BE6-271C-40A6-B94C-C0919520638F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador de proyectos" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Cronograma de proyecto" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ActualBeyond">PeriodInActual*('Planificador de proyectos'!$E1&gt;0)</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -221,13 +222,7 @@
     <t>Flores Bryan</t>
   </si>
   <si>
-    <t>Fernando Fuentes</t>
-  </si>
-  <si>
     <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hito 1. </t>
   </si>
   <si>
     <t>Laurel Gabriela</t>
@@ -253,9 +248,6 @@
     <t>X </t>
   </si>
   <si>
-    <t>Grupo 3</t>
-  </si>
-  <si>
     <t>Manrique Cesar
 Laurel Gabriela</t>
   </si>
@@ -276,19 +268,31 @@
   </si>
   <si>
     <t>PWCEV - CRONOGRAMA DE PROYECTO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Promedio realizado:</t>
+  </si>
+  <si>
+    <t>Fernando Fuentes             Bryan Flores</t>
+  </si>
+  <si>
+    <t>Hito 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -541,6 +545,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1043,7 +1054,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1062,15 +1073,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="7">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1100,42 +1102,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1174,9 +1140,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,9 +1156,60 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="59">
-    <cellStyle name="% completado" xfId="16"/>
+    <cellStyle name="% completado" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20% - Énfasis1" xfId="36" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="40" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="44" builtinId="38" customBuiltin="1"/>
@@ -1214,16 +1228,16 @@
     <cellStyle name="60% - Énfasis4" xfId="50" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="54" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="58" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Actividad" xfId="2"/>
+    <cellStyle name="Actividad" xfId="2" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Bueno" xfId="24" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="29" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="31" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="30" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Control del periodo resaltado" xfId="7"/>
+    <cellStyle name="Control del periodo resaltado" xfId="7" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Encabezados de los periodos" xfId="3"/>
-    <cellStyle name="Encabezados del proyecto" xfId="4"/>
+    <cellStyle name="Encabezados de los periodos" xfId="3" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Encabezados del proyecto" xfId="4" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Énfasis1" xfId="35" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="39" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Énfasis3" xfId="43" builtinId="37" customBuiltin="1"/>
@@ -1231,12 +1245,12 @@
     <cellStyle name="Énfasis5" xfId="51" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="55" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="27" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Etiqueta" xfId="5"/>
+    <cellStyle name="Etiqueta" xfId="5" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Incorrecto" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Leyenda de la duración real" xfId="15"/>
-    <cellStyle name="Leyenda de la duración real (fuera del plan)" xfId="17"/>
-    <cellStyle name="Leyenda del % completado (fuera del plan)" xfId="18"/>
-    <cellStyle name="Leyenda del plan" xfId="14"/>
+    <cellStyle name="Leyenda de la duración real" xfId="15" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Leyenda de la duración real (fuera del plan)" xfId="17" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Leyenda del % completado (fuera del plan)" xfId="18" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Leyenda del plan" xfId="14" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Millares" xfId="19" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Millares [0]" xfId="20" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Moneda" xfId="21" builtinId="4" customBuiltin="1"/>
@@ -1245,7 +1259,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Notas" xfId="33" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Porcentaje" xfId="23" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Porcentaje completado" xfId="6"/>
+    <cellStyle name="Porcentaje completado" xfId="6" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="Salida" xfId="28" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de advertencia" xfId="32" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="12" builtinId="53" customBuiltin="1"/>
@@ -1253,7 +1267,7 @@
     <cellStyle name="Título 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="34" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Valor del periodo" xfId="13"/>
+    <cellStyle name="Valor del periodo" xfId="13" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1637,21 +1651,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA21"/>
+  <dimension ref="B1:AA22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
@@ -1663,103 +1677,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="B1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="11">
         <v>1</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="27" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="27" t="s">
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="19" t="s">
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="30"/>
-    </row>
-    <row r="3" spans="2:27" s="11" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="42"/>
+    </row>
+    <row r="3" spans="2:27" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1822,357 +1836,365 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="48">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="48">
         <v>2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="48">
         <v>2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="48">
         <v>1</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="48">
         <v>1</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="48">
         <v>3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="48">
         <v>2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="48">
         <v>2</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="48">
         <v>2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="48">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="48">
         <v>2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="48">
         <v>1</v>
       </c>
-      <c r="G7" s="7">
-        <v>0.35</v>
+      <c r="G7" s="49">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="48">
         <v>3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="48">
         <v>1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="48">
         <v>3</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="48">
         <v>1</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:27" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="48">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="48">
         <v>2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="48">
         <v>4</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="48">
+        <v>2</v>
+      </c>
+      <c r="G9" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="48">
+        <v>4</v>
+      </c>
+      <c r="D10" s="48">
+        <v>3</v>
+      </c>
+      <c r="E10" s="48">
+        <v>4</v>
+      </c>
+      <c r="F10" s="48">
+        <v>3</v>
+      </c>
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="48">
+        <v>5</v>
+      </c>
+      <c r="D11" s="48">
+        <v>4</v>
+      </c>
+      <c r="E11" s="48">
+        <v>5</v>
+      </c>
+      <c r="F11" s="48">
+        <v>4</v>
+      </c>
+      <c r="G11" s="49">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="48">
+        <v>5</v>
+      </c>
+      <c r="D12" s="48">
+        <v>3</v>
+      </c>
+      <c r="E12" s="48">
+        <v>5</v>
+      </c>
+      <c r="F12" s="48">
+        <v>3</v>
+      </c>
+      <c r="G12" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="48">
+        <v>5</v>
+      </c>
+      <c r="D13" s="48">
+        <v>1</v>
+      </c>
+      <c r="E13" s="48">
+        <v>5</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="48">
+        <v>6</v>
+      </c>
+      <c r="D14" s="48">
+        <v>5</v>
+      </c>
+      <c r="E14" s="48">
+        <v>6</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="50">
+        <v>6</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="48">
+        <v>5</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="48">
+        <v>9</v>
+      </c>
+      <c r="D16" s="48">
+        <v>3</v>
+      </c>
+      <c r="E16" s="48">
+        <v>9</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="48">
+        <v>9</v>
+      </c>
+      <c r="D17" s="48">
+        <v>6</v>
+      </c>
+      <c r="E17" s="48">
+        <v>9</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="48">
+        <v>9</v>
+      </c>
+      <c r="D18" s="48">
+        <v>3</v>
+      </c>
+      <c r="E18" s="48">
+        <v>9</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="48">
+        <v>9</v>
+      </c>
+      <c r="D19" s="48">
+        <v>4</v>
+      </c>
+      <c r="E19" s="48">
         <v>8</v>
       </c>
-      <c r="G9" s="7">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6">
-        <v>3</v>
-      </c>
-      <c r="E10" s="6">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6">
-        <v>6</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="11" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6">
+      <c r="F19" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="48">
+        <v>10</v>
+      </c>
+      <c r="D20" s="48">
         <v>5</v>
       </c>
-      <c r="D11" s="6">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6">
-        <v>5</v>
-      </c>
-      <c r="F11" s="6">
-        <v>3</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:27" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6">
-        <v>5</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="E20" s="48">
+        <v>10</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="48">
+        <v>11</v>
+      </c>
+      <c r="D21" s="48">
         <v>2</v>
       </c>
-      <c r="E12" s="6">
-        <v>5</v>
-      </c>
-      <c r="F12" s="6">
-        <v>5</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6">
-        <v>6</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6">
-        <v>5</v>
-      </c>
-      <c r="E14" s="6">
-        <v>6</v>
-      </c>
-      <c r="F14" s="6">
-        <v>7</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:27" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="8">
-        <v>6</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>5</v>
-      </c>
-      <c r="F15" s="6">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:27" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6">
-        <v>9</v>
-      </c>
-      <c r="D16" s="6">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6">
-        <v>3</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="E21" s="48">
+        <v>11</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="49">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="6">
-        <v>9</v>
-      </c>
-      <c r="D17" s="6">
-        <v>6</v>
-      </c>
-      <c r="E17" s="6">
-        <v>9</v>
-      </c>
-      <c r="F17" s="6">
-        <v>7</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="6">
-        <v>9</v>
-      </c>
-      <c r="D18" s="6">
-        <v>3</v>
-      </c>
-      <c r="E18" s="6">
-        <v>9</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="6">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6">
-        <v>8</v>
-      </c>
-      <c r="F19" s="6">
-        <v>5</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="6">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6">
-        <v>10</v>
-      </c>
-      <c r="F20" s="6">
-        <v>3</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="6">
-        <v>11</v>
-      </c>
-      <c r="D21" s="6">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6">
-        <v>11</v>
-      </c>
-      <c r="F21" s="6">
-        <v>5</v>
-      </c>
-      <c r="G21" s="7">
-        <v>0</v>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:AA2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:AA2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:AA21">
     <cfRule type="expression" dxfId="9" priority="1">
@@ -2211,22 +2233,22 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El planificador de proyectos usa periodos para los intervalos. Inicio = 1 es el periodo 1 y la duración = 5 significa que el proyecto dura 5 periodos desde el periodo de inicio. Introduzca datos a partir de la celda B5 para actualizar el gráfico." sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Escriba un valor del 1 al 60 o seleccione un periodo de la lista (presione CANCELAR, ALT+FLECHA ABAJO y, a continuación, presione ENTRAR para seleccionar un valor)." prompt="Escriba un periodo en el intervalo de 1 a 60 o seleccione un periodo de la lista. Presione ALT+FLECHA ABAJO para desplazarse a la lista y, después, presione ENTRAR para seleccionar un valor." sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El planificador de proyectos usa periodos para los intervalos. Inicio = 1 es el periodo 1 y la duración = 5 significa que el proyecto dura 5 periodos desde el periodo de inicio. Introduzca datos a partir de la celda B5 para actualizar el gráfico." sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Escriba un valor del 1 al 60 o seleccione un periodo de la lista (presione CANCELAR, ALT+FLECHA ABAJO y, a continuación, presione ENTRAR para seleccionar un valor)." prompt="Escriba un periodo en el intervalo de 1 a 60 o seleccione un periodo de la lista. Presione ALT+FLECHA ABAJO para desplazarse a la lista y, después, presione ENTRAR para seleccionar un valor." sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica la duración del plan" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica la duración real" sqref="Q2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado" sqref="V2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Los periodos se representan del 1 al 60, desde la celda H4 a la celda BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la actividad en la columna B, a partir de la celda B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de inicio del plan en la columna C, a partir de la celda C5." sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de duración del plan en la columna D, a partir de la celda D5." sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de inicio real del plan en la columna E, a partir de la celda E5." sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de duración real del plan en la columna F, a partir de la celda F5." sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el porcentaje de proyecto completado en la columna G, a partir de la celda G5." sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Título del proyecto. Escriba un nuevo título en esta celda. Resalte un periodo en H2. La leyenda del gráfico está en las celdas J2 a AI2." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione un período para resaltar en H2. La leyenda de un gráfico está en las celdas J2 a AI2." sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica la duración del plan" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica la duración real" sqref="Q2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta celda de la leyenda indica el porcentaje del proyecto completado" sqref="V2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Los periodos se representan del 1 al 60, desde la celda H4 a la celda BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la actividad en la columna B, a partir de la celda B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de inicio del plan en la columna C, a partir de la celda C5." sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de duración del plan en la columna D, a partir de la celda D5." sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de inicio real del plan en la columna E, a partir de la celda E5." sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el periodo de duración real del plan en la columna F, a partir de la celda F5." sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el porcentaje de proyecto completado en la columna G, a partir de la celda G5." sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Título del proyecto. Escriba un nuevo título en esta celda. Resalte un periodo en H2. La leyenda del gráfico está en las celdas J2 a AI2." sqref="B1" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione un período para resaltar en H2. La leyenda de un gráfico está en las celdas J2 a AI2." sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -2243,642 +2265,645 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
     </row>
     <row r="5" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="38" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="38" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
     </row>
     <row r="8" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-    </row>
-    <row r="9" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:14" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="38" t="s">
+      <c r="G9" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+    </row>
+    <row r="11" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+    </row>
+    <row r="12" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+    </row>
+    <row r="13" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-    </row>
-    <row r="11" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="36" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+    </row>
+    <row r="15" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+    </row>
+    <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+    </row>
+    <row r="17" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+    </row>
+    <row r="18" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-    </row>
-    <row r="12" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-    </row>
-    <row r="13" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+    </row>
+    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+    </row>
+    <row r="20" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15" spans="1:14" ht="57" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="40" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-    </row>
-    <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="40" t="s">
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-    </row>
-    <row r="17" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-    </row>
-    <row r="18" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-    </row>
-    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-    </row>
-    <row r="20" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="36" t="s">
+      <c r="M21" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="28"/>
+    </row>
+    <row r="22" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="L20" s="43" t="s">
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="36" t="s">
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="N21" s="43"/>
-    </row>
-    <row r="22" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="36" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+    </row>
+    <row r="26" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+    </row>
+    <row r="27" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="49" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+    </row>
+    <row r="28" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-    </row>
-    <row r="26" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-    </row>
-    <row r="27" spans="1:14" ht="66" x14ac:dyDescent="0.3">
-      <c r="A27" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-    </row>
-    <row r="28" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2887,5 +2912,6 @@
     <mergeCell ref="A23:N23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificación del cronograma según hitos.
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3041BE6-271C-40A6-B94C-C0919520638F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F1A45-47F0-4E58-8D81-E309F0621B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,8 +28,14 @@
     <definedName name="TitleRegion..BO60">'Planificador de proyectos'!$B$3:$B$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Planificador de proyectos'!$3:$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -233,18 +239,11 @@
 Fuentes Fernando</t>
   </si>
   <si>
-    <t>Hito 2.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manrique Cesar
 Laurel Gabriela
 </t>
   </si>
   <si>
-    <t>Grupo 3
-Lenis Wong</t>
-  </si>
-  <si>
     <t>X </t>
   </si>
   <si>
@@ -252,9 +251,6 @@
 Laurel Gabriela</t>
   </si>
   <si>
-    <t>Hito 3</t>
-  </si>
-  <si>
     <t>Leyenda</t>
   </si>
   <si>
@@ -279,7 +275,47 @@
     <t>Fernando Fuentes             Bryan Flores</t>
   </si>
   <si>
-    <t>Hito 1</t>
+    <t>Creación del documento de arquitectura</t>
+  </si>
+  <si>
+    <t>Loza Piero</t>
+  </si>
+  <si>
+    <t>Entrega de código fuente (Frontend y Backend)</t>
+  </si>
+  <si>
+    <t>Grupo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validación del producto por el cliente</t>
+  </si>
+  <si>
+    <t>Manrique Cesar
+Lenis Wong</t>
+  </si>
+  <si>
+    <t>Creación de Documento de Especificación de Requerimientos</t>
+  </si>
+  <si>
+    <t>Creación del Documento de Arquitectura</t>
+  </si>
+  <si>
+    <t>Documento de solicitud de cambios</t>
+  </si>
+  <si>
+    <t>Validación del producto por el cliente</t>
+  </si>
+  <si>
+    <t>Hito 2: Desarrollo</t>
+  </si>
+  <si>
+    <t>Hito 3: Testing y Despliegue</t>
+  </si>
+  <si>
+    <t>Hito 4: Gestión de Cambios y Configuración</t>
+  </si>
+  <si>
+    <t>Hito 1: Planificación y Documentación</t>
   </si>
 </sst>
 </file>
@@ -1156,6 +1192,18 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1193,18 +1241,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1656,10 +1692,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA22"/>
+  <dimension ref="B1:AA26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1678,7 +1714,7 @@
   <sheetData>
     <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1687,13 +1723,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1701,47 +1737,47 @@
         <v>1</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="43"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
       <c r="V2" s="14"/>
-      <c r="W2" s="40" t="s">
+      <c r="W2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="42"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="46"/>
     </row>
     <row r="3" spans="2:27" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1768,12 +1804,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1839,19 +1875,19 @@
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="35">
         <v>2</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="35">
         <v>2</v>
       </c>
-      <c r="F5" s="48">
+      <c r="F5" s="35">
         <v>1</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="36">
         <v>1</v>
       </c>
     </row>
@@ -1859,19 +1895,19 @@
       <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="35">
         <v>1</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="35">
         <v>3</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="35">
         <v>2</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="35">
         <v>2</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="36">
         <v>1</v>
       </c>
     </row>
@@ -1879,19 +1915,19 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="35">
         <v>2</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="35">
         <v>1</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="35">
         <v>2</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="35">
         <v>1</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="36">
         <v>1</v>
       </c>
     </row>
@@ -1899,287 +1935,367 @@
       <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="35">
         <v>3</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="35">
         <v>1</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="35">
         <v>3</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="35">
         <v>1</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G8" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:27" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="2:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="35">
+        <v>3</v>
+      </c>
+      <c r="D9" s="35">
+        <v>1</v>
+      </c>
+      <c r="E9" s="35">
+        <v>3</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C10" s="35">
         <v>4</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D10" s="35">
         <v>2</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E10" s="35">
         <v>4</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F10" s="35">
         <v>2</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G10" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C11" s="35">
         <v>4</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D11" s="35">
         <v>3</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E11" s="35">
         <v>4</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F11" s="35">
         <v>3</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G11" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+    <row r="12" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C12" s="35">
         <v>5</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D12" s="35">
         <v>4</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E12" s="35">
         <v>5</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F12" s="35">
         <v>4</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G12" s="36">
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+    <row r="13" spans="2:27" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C13" s="35">
         <v>5</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D13" s="35">
         <v>3</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E13" s="35">
         <v>5</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F13" s="35">
         <v>3</v>
       </c>
-      <c r="G12" s="49">
+      <c r="G13" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+    <row r="14" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C14" s="35">
         <v>5</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D14" s="35">
         <v>1</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E14" s="35">
         <v>5</v>
       </c>
-      <c r="F13" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="49">
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+    <row r="15" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C15" s="35">
         <v>6</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D15" s="35">
         <v>5</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E15" s="35">
         <v>6</v>
       </c>
-      <c r="F14" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="49">
+      <c r="F15" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:27" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+    <row r="16" spans="2:27" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C16" s="37">
         <v>6</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D16" s="35">
         <v>1</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E16" s="35">
         <v>5</v>
       </c>
-      <c r="F15" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="49">
+      <c r="F16" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:27" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+    <row r="17" spans="2:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C17" s="35">
         <v>9</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D17" s="35">
         <v>3</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E17" s="35">
         <v>9</v>
       </c>
-      <c r="F16" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="49">
+      <c r="F17" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="2:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C18" s="35">
         <v>9</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D18" s="35">
         <v>6</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E18" s="35">
         <v>9</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="49">
+      <c r="F18" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C19" s="35">
         <v>9</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D19" s="35">
         <v>3</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E19" s="35">
         <v>9</v>
       </c>
-      <c r="F18" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="49">
+      <c r="F19" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+    <row r="20" spans="2:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C20" s="35">
         <v>9</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D20" s="35">
         <v>4</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E20" s="35">
         <v>8</v>
       </c>
-      <c r="F19" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="48">
-        <v>10</v>
-      </c>
-      <c r="D20" s="48">
-        <v>5</v>
-      </c>
-      <c r="E20" s="48">
-        <v>10</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="49">
+      <c r="F20" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="35">
+        <v>10</v>
+      </c>
+      <c r="D21" s="35">
+        <v>5</v>
+      </c>
+      <c r="E21" s="35">
+        <v>10</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C22" s="35">
         <v>11</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D22" s="35">
         <v>2</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E22" s="35">
         <v>11</v>
       </c>
-      <c r="F21" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="49">
+      <c r="F22" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="4">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="35">
+        <v>10</v>
+      </c>
+      <c r="D23" s="35">
+        <v>1</v>
+      </c>
+      <c r="E23" s="35">
+        <v>10</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="35">
+        <v>10</v>
+      </c>
+      <c r="D24" s="35">
+        <v>2</v>
+      </c>
+      <c r="E24" s="35">
+        <v>10</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="35">
+        <v>12</v>
+      </c>
+      <c r="D25" s="35">
+        <v>1</v>
+      </c>
+      <c r="E25" s="35">
+        <v>12</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="4">
         <v>0.45</v>
       </c>
     </row>
@@ -2196,7 +2312,7 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:AA21">
+  <conditionalFormatting sqref="H5:AA25">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PorcentajeCompletado</formula>
     </cfRule>
@@ -2222,7 +2338,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:AA22">
+  <conditionalFormatting sqref="B26:AA26">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -2266,10 +2382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2355,7 +2471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2377,7 +2493,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2423,7 +2539,7 @@
     </row>
     <row r="7" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>48</v>
@@ -2444,108 +2560,104 @@
       <c r="N7" s="26"/>
     </row>
     <row r="8" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B9" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:14" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-    </row>
-    <row r="11" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="10" spans="1:14" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+    </row>
+    <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B12" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="23" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
       <c r="E12" s="23" t="s">
         <v>50</v>
       </c>
@@ -2558,21 +2670,23 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="21"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
-      <c r="E13" s="28"/>
+      <c r="E13" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="F13" s="23" t="s">
         <v>50</v>
       </c>
@@ -2580,68 +2694,70 @@
         <v>50</v>
       </c>
       <c r="H13" s="22"/>
-      <c r="I13" s="29"/>
+      <c r="I13" s="22"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-    </row>
-    <row r="15" spans="1:14" ht="57" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="28" t="s">
+    <row r="14" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
+      <c r="G14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
     </row>
     <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="28" t="s">
+      <c r="G16" s="28" t="s">
         <v>50</v>
       </c>
+      <c r="H16" s="30"/>
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
@@ -2649,36 +2765,34 @@
       <c r="M16" s="30"/>
       <c r="N16" s="30"/>
     </row>
-    <row r="17" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+    </row>
+    <row r="18" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B18" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-    </row>
-    <row r="18" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>46</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
@@ -2697,55 +2811,55 @@
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
     </row>
-    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="28" t="s">
-        <v>50</v>
-      </c>
+      <c r="H19" s="30"/>
       <c r="I19" s="28" t="s">
         <v>50</v>
       </c>
       <c r="J19" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="K19" s="28" t="s">
-        <v>50</v>
-      </c>
+      <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="H20" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>50</v>
+      </c>
       <c r="K20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="L20" s="28" t="s">
-        <v>56</v>
-      </c>
+      <c r="L20" s="28"/>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
     </row>
@@ -2770,7 +2884,7 @@
         <v>50</v>
       </c>
       <c r="L21" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M21" s="28" t="s">
         <v>50</v>
@@ -2782,7 +2896,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -2796,101 +2910,114 @@
       <c r="L22" s="31"/>
       <c r="M22" s="32"/>
       <c r="N22" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-    </row>
-    <row r="26" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-    </row>
-    <row r="27" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-    </row>
-    <row r="28" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
-        <v>62</v>
-      </c>
+      <c r="A23" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+    </row>
+    <row r="24" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+    </row>
+    <row r="25" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="28"/>
+    </row>
+    <row r="26" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -2905,11 +3032,75 @@
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
     </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A14:N14"/>
+  <mergeCells count="4">
+    <mergeCell ref="A11:N11"/>
+    <mergeCell ref="A15:N15"/>
     <mergeCell ref="A23:N23"/>
+    <mergeCell ref="A27:N27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de cronograma v3
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F1A45-47F0-4E58-8D81-E309F0621B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C5C955-0D27-4203-AA40-5F9AAF7128A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador de proyectos" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -115,9 +115,6 @@
     <t xml:space="preserve"> Modelamiento de la BD </t>
   </si>
   <si>
-    <t xml:space="preserve"> Desarrollo de vistas (frontend)</t>
-  </si>
-  <si>
     <t>Levantamiento de backend y despliegue a servirdor</t>
   </si>
   <si>
@@ -130,22 +127,7 @@
     <t xml:space="preserve">Integración de Algoritmo antiplagio </t>
   </si>
   <si>
-    <t>Creación y almacenamiento de respuestas de exámenes</t>
-  </si>
-  <si>
-    <t>CRUD de respuestas, cursos y exámenes de la vista Docente</t>
-  </si>
-  <si>
-    <t>Pruebas funcionales</t>
-  </si>
-  <si>
-    <t>Gestión de cambios del proyecto</t>
-  </si>
-  <si>
     <t>Testing </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Despliegue a producción</t>
   </si>
   <si>
     <t>INICIO DEL PLAN
@@ -316,6 +298,51 @@
   </si>
   <si>
     <t>Hito 1: Planificación y Documentación</t>
+  </si>
+  <si>
+    <t>Validación de usuarios por tokens</t>
+  </si>
+  <si>
+    <t>Fuentes Fernando</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desarrollo de vistas (frontend - Docente)</t>
+  </si>
+  <si>
+    <t>Levantamiento de backend y despliegue a servidor</t>
+  </si>
+  <si>
+    <t>Creación de API's de cursos y usuarios</t>
+  </si>
+  <si>
+    <t>Creación de API's de cursos y usuarios (Front y Back)</t>
+  </si>
+  <si>
+    <t>Fuentes Fernando Laurel Gabriela</t>
+  </si>
+  <si>
+    <t>CRUD de respuestas y exámenes de la vista Docente</t>
+  </si>
+  <si>
+    <t>Optimización de código</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Segunda presentación del sistema a la gerente</t>
+  </si>
+  <si>
+    <t>Primera presentación del sistema a la gerente</t>
+  </si>
+  <si>
+    <t>Creación de API de  exámenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desarrollo de vistas (frontend - Alumno)</t>
+  </si>
+  <si>
+    <t>Creación de Api de exámenes</t>
+  </si>
+  <si>
+    <t>Desarrollo de vistas (Fronted - Alumno)</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1242,6 +1269,9 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1692,10 +1722,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA26"/>
+  <dimension ref="B1:AA27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1714,7 +1744,7 @@
   <sheetData>
     <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1766,16 +1796,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>2</v>
@@ -1953,7 +1983,7 @@
     </row>
     <row r="9" spans="2:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C9" s="35">
         <v>3</v>
@@ -2013,7 +2043,7 @@
     </row>
     <row r="12" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C12" s="35">
         <v>5</v>
@@ -2033,7 +2063,7 @@
     </row>
     <row r="13" spans="2:27" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="35">
         <v>5</v>
@@ -2053,199 +2083,199 @@
     </row>
     <row r="14" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="35">
+        <v>4</v>
+      </c>
+      <c r="D14" s="35">
+        <v>2</v>
+      </c>
+      <c r="E14" s="35">
+        <v>4</v>
+      </c>
+      <c r="F14" s="35">
+        <v>5</v>
+      </c>
+      <c r="G14" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="35">
+        <v>5</v>
+      </c>
+      <c r="D15" s="35">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35">
+        <v>5</v>
+      </c>
+      <c r="F15" s="35">
+        <v>2</v>
+      </c>
+      <c r="G15" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="35">
+        <v>7</v>
+      </c>
+      <c r="D16" s="35">
+        <v>2</v>
+      </c>
+      <c r="E16" s="35">
+        <v>7</v>
+      </c>
+      <c r="F16" s="35">
+        <v>2</v>
+      </c>
+      <c r="G16" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C17" s="35">
         <v>5</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D17" s="35">
         <v>1</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E17" s="35">
         <v>5</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="35">
+      <c r="F17" s="35">
+        <v>1</v>
+      </c>
+      <c r="G17" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="35">
         <v>6</v>
       </c>
-      <c r="D15" s="35">
-        <v>5</v>
-      </c>
-      <c r="E15" s="35">
+      <c r="D18" s="35">
+        <v>2</v>
+      </c>
+      <c r="E18" s="35">
         <v>6</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:27" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
+      <c r="F18" s="35">
+        <v>2</v>
+      </c>
+      <c r="G18" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="35">
+        <v>8</v>
+      </c>
+      <c r="D19" s="35">
+        <v>2</v>
+      </c>
+      <c r="E19" s="35">
+        <v>8</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="36">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="37">
-        <v>6</v>
-      </c>
-      <c r="D16" s="35">
-        <v>1</v>
-      </c>
-      <c r="E16" s="35">
-        <v>5</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="35">
-        <v>9</v>
-      </c>
-      <c r="D17" s="35">
-        <v>3</v>
-      </c>
-      <c r="E17" s="35">
-        <v>9</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="35">
-        <v>9</v>
-      </c>
-      <c r="D18" s="35">
-        <v>6</v>
-      </c>
-      <c r="E18" s="35">
-        <v>9</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="35">
-        <v>9</v>
-      </c>
-      <c r="D19" s="35">
-        <v>3</v>
-      </c>
-      <c r="E19" s="35">
-        <v>9</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
-        <v>22</v>
-      </c>
       <c r="C20" s="35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E20" s="35">
         <v>8</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G20" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
-        <v>23</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C21" s="35">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D21" s="35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" s="35">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G21" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18" t="s">
-        <v>24</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="C22" s="35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D22" s="35">
         <v>2</v>
       </c>
       <c r="E22" s="35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G22" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="35">
-        <v>10</v>
+    <row r="23" spans="2:7" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="37">
+        <v>9</v>
       </c>
       <c r="D23" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="35">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G23" s="36">
         <v>0</v>
@@ -2253,19 +2283,19 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C24" s="35">
         <v>10</v>
       </c>
       <c r="D24" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="35">
         <v>10</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G24" s="36">
         <v>0</v>
@@ -2273,30 +2303,50 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C25" s="35">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="35">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G25" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="4">
-        <v>0.45</v>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="35">
+        <v>12</v>
+      </c>
+      <c r="D26" s="35">
+        <v>1</v>
+      </c>
+      <c r="E26" s="35">
+        <v>12</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -2312,7 +2362,7 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:AA25">
+  <conditionalFormatting sqref="H5:AA26">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PorcentajeCompletado</formula>
     </cfRule>
@@ -2338,7 +2388,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:AA26">
+  <conditionalFormatting sqref="B27:AA27">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -2382,10 +2432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:N11"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,7 +2445,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -2429,46 +2479,46 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="H3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="K3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="N3" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2476,11 +2526,11 @@
         <v>8</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -2498,11 +2548,11 @@
         <v>9</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -2520,11 +2570,11 @@
         <v>10</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
@@ -2539,15 +2589,15 @@
     </row>
     <row r="7" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="27"/>
       <c r="E7" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
@@ -2561,15 +2611,15 @@
     </row>
     <row r="8" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="27"/>
       <c r="E8" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
@@ -2586,11 +2636,11 @@
         <v>12</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
@@ -2608,18 +2658,18 @@
         <v>13</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="28"/>
       <c r="E10" s="23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -2631,7 +2681,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="51" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -2649,26 +2699,30 @@
     </row>
     <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22"/>
       <c r="L12" s="21"/>
@@ -2677,21 +2731,21 @@
     </row>
     <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -2703,19 +2757,19 @@
     </row>
     <row r="14" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="28"/>
       <c r="F14" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="29"/>
@@ -2725,150 +2779,148 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-    </row>
-    <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-    </row>
-    <row r="17" spans="1:14" ht="57" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-    </row>
-    <row r="18" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+    <row r="15" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+    </row>
+    <row r="18" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="H18" s="30"/>
-      <c r="I18" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="30"/>
+      <c r="H19" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="I19" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>50</v>
-      </c>
+    <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K20" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
@@ -2878,25 +2930,21 @@
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
       <c r="J21" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K21" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="L21" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="M21" s="28" t="s">
-        <v>50</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L21" s="30"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="28"/>
     </row>
     <row r="22" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -2905,84 +2953,92 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
+      <c r="J22" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="K22" s="28"/>
-      <c r="L22" s="31"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="32"/>
-      <c r="N22" s="28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-    </row>
-    <row r="24" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
-        <v>66</v>
+      <c r="N22" s="28"/>
+    </row>
+    <row r="23" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="30"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+    </row>
+    <row r="24" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-    </row>
-    <row r="25" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="21"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+    </row>
+    <row r="26" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="M25" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="N25" s="28"/>
-    </row>
-    <row r="26" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
@@ -2993,15 +3049,15 @@
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
-      <c r="L26" s="31"/>
+      <c r="L26" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="M26" s="32"/>
-      <c r="N26" s="28" t="s">
-        <v>54</v>
-      </c>
+      <c r="N26" s="28"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="51" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
@@ -3017,90 +3073,176 @@
       <c r="M27" s="51"/>
       <c r="N27" s="51"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+    <row r="28" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+    </row>
+    <row r="29" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29" s="28"/>
+    </row>
+    <row r="30" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="28" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="A31" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
-        <v>59</v>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A11:N11"/>
-    <mergeCell ref="A15:N15"/>
-    <mergeCell ref="A23:N23"/>
+    <mergeCell ref="A17:N17"/>
     <mergeCell ref="A27:N27"/>
+    <mergeCell ref="A31:N31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de porcentaje de proyecto completado.
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Project\WebSecurity\WebSecurity\DESARROLLO\PWCEV\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C5C955-0D27-4203-AA40-5F9AAF7128A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051864AA-BC15-4724-AA40-793188DA03DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1231,6 +1231,9 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1269,9 +1272,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1753,13 +1753,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1767,47 +1767,47 @@
         <v>1</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="14"/>
-      <c r="W2" s="44" t="s">
+      <c r="W2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="46"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="47"/>
     </row>
     <row r="3" spans="2:27" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="40" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1834,12 +1834,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="49"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>55</v>
       </c>
       <c r="G20" s="36">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2346,7 +2346,8 @@
         <v>56</v>
       </c>
       <c r="G27" s="4">
-        <v>0.7</v>
+        <f>AVERAGE(G5:G26)</f>
+        <v>0.68181818181818177</v>
       </c>
     </row>
   </sheetData>
@@ -2680,22 +2681,22 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
     </row>
     <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
@@ -2786,9 +2787,9 @@
       <c r="B15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
         <v>44</v>
@@ -2796,8 +2797,8 @@
       <c r="H15" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="18"/>
@@ -2815,7 +2816,7 @@
       <c r="E16" s="28"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="52"/>
+      <c r="H16" s="39"/>
       <c r="I16" s="23" t="s">
         <v>44</v>
       </c>
@@ -2828,22 +2829,22 @@
       <c r="N16" s="18"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
     </row>
     <row r="18" spans="1:14" ht="57" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
@@ -2885,8 +2886,8 @@
       <c r="I19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
@@ -3056,22 +3057,22 @@
       <c r="N26" s="28"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
     </row>
     <row r="28" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
@@ -3142,22 +3143,22 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" s="19"/>

</xml_diff>

<commit_message>
Actualización de cronograma v3 y bitácora de incidencias.
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Project\WebSecurity\WebSecurity\DESARROLLO\PWCEV\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Web Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051864AA-BC15-4724-AA40-793188DA03DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E8F447-05A7-479D-91E8-E34586B891DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,12 +30,6 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -44,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -127,9 +121,6 @@
     <t xml:space="preserve">Integración de Algoritmo antiplagio </t>
   </si>
   <si>
-    <t>Testing </t>
-  </si>
-  <si>
     <t>INICIO DEL PLAN
 (SEMANA)</t>
   </si>
@@ -282,9 +273,6 @@
     <t>Creación del Documento de Arquitectura</t>
   </si>
   <si>
-    <t>Documento de solicitud de cambios</t>
-  </si>
-  <si>
     <t>Validación del producto por el cliente</t>
   </si>
   <si>
@@ -343,6 +331,25 @@
   </si>
   <si>
     <t>Desarrollo de vistas (Fronted - Alumno)</t>
+  </si>
+  <si>
+    <t>Despliegue a servidor de prueba</t>
+  </si>
+  <si>
+    <t>Testing (pruebas estáticas)</t>
+  </si>
+  <si>
+    <t>Testing (pruebas funcionales)</t>
+  </si>
+  <si>
+    <t>Laurel Gabriela Fuentes Fernando</t>
+  </si>
+  <si>
+    <t>Testing (pruebas estáticas)</t>
+  </si>
+  <si>
+    <t>Manrique Cesar
+Laurel Gabriela Flores Bryan</t>
   </si>
 </sst>
 </file>
@@ -355,7 +362,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -616,8 +623,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -835,6 +847,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,7 +1135,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1209,7 +1227,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1273,6 +1290,32 @@
     <xf numFmtId="0" fontId="34" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="% completado" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1722,10 +1765,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA27"/>
+  <dimension ref="B1:AA28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1744,7 +1787,7 @@
   <sheetData>
     <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1753,13 +1796,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1767,47 +1810,47 @@
         <v>1</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="44"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="43"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="42" t="s">
+      <c r="R2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="44"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
       <c r="V2" s="14"/>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="47"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="46"/>
     </row>
     <row r="3" spans="2:27" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="51" t="s">
+      <c r="F3" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1834,12 +1877,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="50"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1905,19 +1948,19 @@
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>2</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="34">
         <v>2</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="34">
         <v>1</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>1</v>
       </c>
     </row>
@@ -1925,19 +1968,19 @@
       <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <v>3</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <v>2</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="34">
         <v>2</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>1</v>
       </c>
     </row>
@@ -1945,19 +1988,19 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="34">
         <v>2</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>1</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="34">
         <v>2</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="34">
         <v>1</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>1</v>
       </c>
     </row>
@@ -1965,39 +2008,39 @@
       <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="34">
         <v>3</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>1</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="34">
         <v>3</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="34">
         <v>1</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="35">
+        <v>64</v>
+      </c>
+      <c r="C9" s="34">
         <v>3</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <v>1</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="34">
         <v>3</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <v>1</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2005,19 +2048,19 @@
       <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>4</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <v>2</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="34">
         <v>4</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <v>2</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2025,39 +2068,39 @@
       <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>4</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <v>3</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <v>4</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <v>3</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:27" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="35">
+        <v>72</v>
+      </c>
+      <c r="C12" s="34">
         <v>5</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <v>4</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="34">
         <v>5</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <v>4</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="35">
         <v>0.6</v>
       </c>
     </row>
@@ -2065,19 +2108,19 @@
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <v>5</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <v>3</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <v>5</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="34">
         <v>3</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2085,59 +2128,59 @@
       <c r="B14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>4</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="34">
         <v>2</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="34">
         <v>4</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="34">
         <v>5</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:27" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="35">
+        <v>74</v>
+      </c>
+      <c r="C15" s="34">
         <v>5</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="34">
         <v>2</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="34">
         <v>5</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="34">
         <v>2</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:27" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="35">
+        <v>70</v>
+      </c>
+      <c r="C16" s="34">
         <v>7</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="34">
         <v>2</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="34">
         <v>7</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="34">
         <v>2</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2145,119 +2188,119 @@
       <c r="B17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="34">
         <v>5</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="34">
         <v>1</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="34">
         <v>5</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="34">
         <v>1</v>
       </c>
-      <c r="G17" s="36">
+      <c r="G17" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="35">
+        <v>77</v>
+      </c>
+      <c r="C18" s="34">
         <v>6</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <v>2</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="34">
         <v>6</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="34">
         <v>2</v>
       </c>
-      <c r="G18" s="36">
+      <c r="G18" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="35">
+        <v>78</v>
+      </c>
+      <c r="C19" s="34">
         <v>8</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="34">
         <v>2</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="34">
         <v>8</v>
       </c>
-      <c r="F19" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="36">
+      <c r="F19" s="34">
+        <v>2</v>
+      </c>
+      <c r="G19" s="35">
         <v>0.7</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="35">
+        <v>89</v>
+      </c>
+      <c r="C20" s="34">
         <v>8</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <v>2</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="34">
         <v>8</v>
       </c>
-      <c r="F20" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="36">
-        <v>0.2</v>
+      <c r="F20" s="34">
+        <v>2</v>
+      </c>
+      <c r="G20" s="35">
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="35">
+        <v>83</v>
+      </c>
+      <c r="C21" s="34">
         <v>8</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <v>2</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="34">
         <v>8</v>
       </c>
-      <c r="F21" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="36">
-        <v>0.5</v>
+      <c r="F21" s="34">
+        <v>2</v>
+      </c>
+      <c r="G21" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="35">
-        <v>8</v>
-      </c>
-      <c r="D22" s="35">
+        <v>84</v>
+      </c>
+      <c r="C22" s="34">
+        <v>9</v>
+      </c>
+      <c r="D22" s="34">
         <v>2</v>
       </c>
-      <c r="E22" s="35">
-        <v>8</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="36">
+      <c r="E22" s="34">
+        <v>9</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="35">
         <v>0</v>
       </c>
     </row>
@@ -2265,89 +2308,109 @@
       <c r="B23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="36">
         <v>9</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="34">
         <v>2</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="34">
         <v>9</v>
       </c>
-      <c r="F23" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="36">
-        <v>0</v>
+      <c r="F23" s="34">
+        <v>2</v>
+      </c>
+      <c r="G23" s="35">
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="35">
+        <v>85</v>
+      </c>
+      <c r="C24" s="34">
         <v>10</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="34">
         <v>1</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="34">
         <v>10</v>
       </c>
-      <c r="F24" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="36">
+      <c r="F24" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="35">
+        <v>87</v>
+      </c>
+      <c r="C25" s="34">
         <v>10</v>
       </c>
-      <c r="D25" s="35">
-        <v>2</v>
-      </c>
-      <c r="E25" s="35">
+      <c r="D25" s="34">
+        <v>1</v>
+      </c>
+      <c r="E25" s="34">
         <v>10</v>
       </c>
-      <c r="F25" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="36">
-        <v>0</v>
+      <c r="F25" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0.4</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="35">
+        <v>59</v>
+      </c>
+      <c r="C26" s="34">
+        <v>11</v>
+      </c>
+      <c r="D26" s="34">
+        <v>2</v>
+      </c>
+      <c r="E26" s="34">
+        <v>11</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="34">
         <v>12</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D27" s="34">
         <v>1</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E27" s="34">
         <v>12</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F27" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="4">
-        <f>AVERAGE(G5:G26)</f>
-        <v>0.68181818181818177</v>
+      <c r="G28" s="4">
+        <f>AVERAGE(G5:G27)</f>
+        <v>0.74782608695652153</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2426,7 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:AA26">
+  <conditionalFormatting sqref="H5:AA27">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PorcentajeCompletado</formula>
     </cfRule>
@@ -2389,7 +2452,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:AA27">
+  <conditionalFormatting sqref="B28:AA28">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -2433,20 +2496,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -2458,7 +2522,7 @@
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="L1" s="53"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
@@ -2474,52 +2538,52 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="C3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="G3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="K3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="N3" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2527,11 +2591,11 @@
         <v>8</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -2540,7 +2604,7 @@
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
@@ -2549,11 +2613,11 @@
         <v>9</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -2562,7 +2626,7 @@
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
     </row>
@@ -2571,11 +2635,11 @@
         <v>10</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
@@ -2584,21 +2648,21 @@
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="L6" s="55"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="27"/>
       <c r="E7" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
@@ -2606,21 +2670,21 @@
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="L7" s="56"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
     </row>
     <row r="8" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="27"/>
       <c r="E8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
@@ -2628,7 +2692,7 @@
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
+      <c r="L8" s="56"/>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
     </row>
@@ -2637,11 +2701,11 @@
         <v>12</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
@@ -2650,7 +2714,7 @@
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
@@ -2659,100 +2723,100 @@
         <v>13</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="28"/>
       <c r="E10" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="L10" s="57"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="A11" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
     </row>
     <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22"/>
-      <c r="L12" s="21"/>
+      <c r="L12" s="57"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="L13" s="57"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
@@ -2761,119 +2825,119 @@
         <v>15</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="28"/>
       <c r="F14" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="29"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
     <row r="15" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+        <v>76</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+        <v>43</v>
+      </c>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
+      <c r="L15" s="57"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
     </row>
     <row r="16" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="28"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="39"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="L16" s="57"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
+      <c r="A17" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
     </row>
     <row r="18" spans="1:14" ht="57" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
     </row>
     <row r="19" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -2881,23 +2945,23 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="59"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
     </row>
     <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -2907,21 +2971,21 @@
       <c r="H20" s="28"/>
       <c r="I20" s="30"/>
       <c r="J20" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K20" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="L20" s="58"/>
       <c r="M20" s="30"/>
       <c r="N20" s="30"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
@@ -2931,21 +2995,21 @@
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
       <c r="J21" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K21" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L21" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="L21" s="58"/>
       <c r="M21" s="28"/>
       <c r="N21" s="28"/>
     </row>
     <row r="22" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -2955,19 +3019,19 @@
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="32"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="28"/>
     </row>
     <row r="23" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
@@ -2977,21 +3041,21 @@
       <c r="H23" s="30"/>
       <c r="I23" s="28"/>
       <c r="J23" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L23" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="L23" s="58"/>
       <c r="M23" s="28"/>
       <c r="N23" s="28"/>
     </row>
     <row r="24" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="23"/>
@@ -3000,13 +3064,12 @@
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
-      <c r="J24" s="28" t="s">
-        <v>44</v>
-      </c>
       <c r="K24" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L24" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="L24" s="59" t="s">
+        <v>43</v>
+      </c>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
     </row>
@@ -3015,7 +3078,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -3025,21 +3088,20 @@
       <c r="H25" s="28"/>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
-      <c r="K25" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="L25" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="M25" s="28"/>
+      <c r="L25" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="30" t="s">
+        <v>43</v>
+      </c>
       <c r="N25" s="28"/>
     </row>
-    <row r="26" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="57" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
@@ -3050,82 +3112,82 @@
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
-      <c r="L26" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="M26" s="32"/>
+      <c r="L26" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="31"/>
       <c r="N26" s="28"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-    </row>
-    <row r="28" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="A27" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+    </row>
+    <row r="28" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
     </row>
     <row r="29" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="M29" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="N29" s="28"/>
+      <c r="A29" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="M29" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="N29" s="52"/>
     </row>
     <row r="30" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
@@ -3136,44 +3198,50 @@
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="52"/>
+      <c r="M30" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="N30" s="28"/>
+    </row>
+    <row r="31" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="28" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="A32" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="51"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B33" s="19"/>
@@ -3186,7 +3254,7 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
+      <c r="L33" s="53"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
     </row>
@@ -3201,14 +3269,11 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
+      <c r="L34" s="53"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="33" t="s">
-        <v>50</v>
-      </c>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -3219,23 +3284,41 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
+      <c r="L35" s="53"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="34" t="s">
+    <row r="39" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="37" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="38" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3243,7 +3326,7 @@
     <mergeCell ref="A11:N11"/>
     <mergeCell ref="A17:N17"/>
     <mergeCell ref="A27:N27"/>
-    <mergeCell ref="A31:N31"/>
+    <mergeCell ref="A32:N32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de bitácora de incidencias y cronograma - presentación
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Web Security\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyectoGestion\WebSecurity\WebSecurity\DESARROLLO\PWCEV\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB98BE-49F3-4D19-84C2-E9EBC04DDF81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE49D7E6-5DE6-4309-B7BE-09F150A4C991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="92">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -351,6 +351,9 @@
     <t>Manrique Cesar
 Laurel Gabriela Flores Bryan</t>
   </si>
+  <si>
+    <t>S13</t>
+  </si>
 </sst>
 </file>
 
@@ -629,7 +632,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -853,6 +856,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1135,7 +1144,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1277,6 +1286,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1768,7 +1783,7 @@
   <dimension ref="B1:AA28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1796,13 +1811,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1810,47 +1825,47 @@
         <v>1</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="53"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="55"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="51" t="s">
+      <c r="R2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="53"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="55"/>
       <c r="V2" s="14"/>
-      <c r="W2" s="54" t="s">
+      <c r="W2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="56"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="58"/>
     </row>
     <row r="3" spans="2:27" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="51" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1877,12 +1892,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="59"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2241,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="35">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2261,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="35">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2301,7 +2316,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="35">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2321,7 +2336,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="35">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,7 +2344,7 @@
         <v>85</v>
       </c>
       <c r="C24" s="34">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D24" s="34">
         <v>2</v>
@@ -2338,10 +2353,10 @@
         <v>10</v>
       </c>
       <c r="F24" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" s="35">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2352,16 +2367,16 @@
         <v>10</v>
       </c>
       <c r="D25" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="34">
         <v>10</v>
       </c>
       <c r="F25" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="35">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2369,19 +2384,19 @@
         <v>59</v>
       </c>
       <c r="C26" s="34">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D26" s="34">
         <v>2</v>
       </c>
       <c r="E26" s="34">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>54</v>
       </c>
       <c r="G26" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2389,19 +2404,19 @@
         <v>65</v>
       </c>
       <c r="C27" s="34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="34">
         <v>1</v>
       </c>
       <c r="E27" s="34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>54</v>
       </c>
       <c r="G27" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2410,7 +2425,7 @@
       </c>
       <c r="G28" s="4">
         <f>AVERAGE(G5:G27)</f>
-        <v>0.79999999999999993</v>
+        <v>0.97826086956521741</v>
       </c>
     </row>
   </sheetData>
@@ -2496,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2508,7 +2523,7 @@
     <col min="12" max="12" width="11.5546875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>22</v>
       </c>
@@ -2526,7 +2541,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -2542,7 +2557,7 @@
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
@@ -2585,8 +2600,11 @@
       <c r="N3" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2607,8 +2625,9 @@
       <c r="L4" s="42"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
-    </row>
-    <row r="5" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2629,8 +2648,9 @@
       <c r="L5" s="42"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
-    </row>
-    <row r="6" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -2651,8 +2671,9 @@
       <c r="L6" s="42"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
-    </row>
-    <row r="7" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>63</v>
       </c>
@@ -2673,8 +2694,9 @@
       <c r="L7" s="43"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O7" s="26"/>
+    </row>
+    <row r="8" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>57</v>
       </c>
@@ -2695,8 +2717,9 @@
       <c r="L8" s="43"/>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="O8" s="26"/>
+    </row>
+    <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
@@ -2717,8 +2740,9 @@
       <c r="L9" s="42"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:14" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" spans="1:15" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
@@ -2743,26 +2767,28 @@
       <c r="L10" s="44"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-    </row>
-    <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="50"/>
+    </row>
+    <row r="12" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>72</v>
       </c>
@@ -2793,8 +2819,9 @@
       <c r="L12" s="44"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>73</v>
       </c>
@@ -2819,8 +2846,9 @@
       <c r="L13" s="44"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
-    </row>
-    <row r="14" spans="1:14" ht="68.400000000000006" x14ac:dyDescent="0.3">
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:15" ht="68.400000000000006" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -2843,8 +2871,9 @@
       <c r="L14" s="44"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="1:15" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>75</v>
       </c>
@@ -2867,8 +2896,9 @@
       <c r="L15" s="44"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>70</v>
       </c>
@@ -2891,26 +2921,28 @@
       <c r="L16" s="44"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="61" t="s">
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-    </row>
-    <row r="18" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="50"/>
+    </row>
+    <row r="18" spans="1:15" ht="57" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -2931,8 +2963,9 @@
       <c r="L18" s="45"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
-    </row>
-    <row r="19" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O18" s="30"/>
+    </row>
+    <row r="19" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>77</v>
       </c>
@@ -2955,8 +2988,9 @@
       <c r="L19" s="46"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
-    </row>
-    <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="O19" s="28"/>
+    </row>
+    <row r="20" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>78</v>
       </c>
@@ -2979,8 +3013,9 @@
       <c r="L20" s="45"/>
       <c r="M20" s="30"/>
       <c r="N20" s="30"/>
-    </row>
-    <row r="21" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="O20" s="30"/>
+    </row>
+    <row r="21" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>86</v>
       </c>
@@ -3003,8 +3038,9 @@
       <c r="L21" s="45"/>
       <c r="M21" s="28"/>
       <c r="N21" s="28"/>
-    </row>
-    <row r="22" spans="1:14" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="O21" s="28"/>
+    </row>
+    <row r="22" spans="1:15" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>80</v>
       </c>
@@ -3025,8 +3061,9 @@
       <c r="L22" s="46"/>
       <c r="M22" s="31"/>
       <c r="N22" s="28"/>
-    </row>
-    <row r="23" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O22" s="28"/>
+    </row>
+    <row r="23" spans="1:15" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>81</v>
       </c>
@@ -3049,8 +3086,9 @@
       <c r="L23" s="45"/>
       <c r="M23" s="28"/>
       <c r="N23" s="28"/>
-    </row>
-    <row r="24" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O23" s="28"/>
+    </row>
+    <row r="24" spans="1:15" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>82</v>
       </c>
@@ -3070,10 +3108,13 @@
       <c r="L24" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="18"/>
+      <c r="M24" s="46" t="s">
+        <v>43</v>
+      </c>
       <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="O24" s="18"/>
+    </row>
+    <row r="25" spans="1:15" ht="57" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>17</v>
       </c>
@@ -3095,8 +3136,9 @@
         <v>43</v>
       </c>
       <c r="N25" s="28"/>
-    </row>
-    <row r="26" spans="1:14" ht="57" x14ac:dyDescent="0.3">
+      <c r="O25" s="28"/>
+    </row>
+    <row r="26" spans="1:15" ht="57" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>79</v>
       </c>
@@ -3112,31 +3154,32 @@
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
-      <c r="L26" s="46" t="s">
+      <c r="M26" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="M26" s="31"/>
       <c r="N26" s="28"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="61" t="s">
+      <c r="O26" s="28"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-    </row>
-    <row r="28" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="50"/>
+    </row>
+    <row r="28" spans="1:15" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>85</v>
       </c>
@@ -3152,15 +3195,16 @@
       <c r="I28" s="39"/>
       <c r="J28" s="39"/>
       <c r="K28" s="39"/>
-      <c r="L28" s="46" t="s">
-        <v>47</v>
-      </c>
+      <c r="L28" s="49"/>
       <c r="M28" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="N28" s="39"/>
-    </row>
-    <row r="29" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="N28" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="O28" s="39"/>
+    </row>
+    <row r="29" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>87</v>
       </c>
@@ -3176,15 +3220,16 @@
       <c r="I29" s="39"/>
       <c r="J29" s="39"/>
       <c r="K29" s="39"/>
-      <c r="L29" s="46" t="s">
+      <c r="L29" s="49"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="M29" s="46" t="s">
+      <c r="O29" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="N29" s="39"/>
-    </row>
-    <row r="30" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>59</v>
       </c>
@@ -3200,12 +3245,14 @@
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
-      <c r="M30" s="46" t="s">
+      <c r="L30" s="49"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="N30" s="28"/>
-    </row>
-    <row r="31" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>61</v>
       </c>
@@ -3221,29 +3268,31 @@
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="28" t="s">
+      <c r="L31" s="49"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="61" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="50"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B33" s="19"/>

</xml_diff>